<commit_message>
create new property completed
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/TestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sukeshkumar/Development/projects/egov/egov_functional_test/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sukeshkumar/Development/projects/egov-functional/eGov/egov/egov_functional_test/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,10 @@
     <sheet name="addressDetails" sheetId="4" r:id="rId3"/>
     <sheet name="assessmentDetails" sheetId="5" r:id="rId4"/>
     <sheet name="amenities" sheetId="6" r:id="rId5"/>
-    <sheet name="propertyHeaderDetails" sheetId="2" r:id="rId6"/>
+    <sheet name="constructionTypeDetails" sheetId="7" r:id="rId6"/>
+    <sheet name="floorDetails" sheetId="8" r:id="rId7"/>
+    <sheet name="approvalDetails" sheetId="9" r:id="rId8"/>
+    <sheet name="propertyHeaderDetails" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="89">
   <si>
     <t>dataName</t>
   </si>
@@ -179,6 +182,126 @@
   </si>
   <si>
     <t>cableConnection</t>
+  </si>
+  <si>
+    <t>floorType</t>
+  </si>
+  <si>
+    <t>roofType</t>
+  </si>
+  <si>
+    <t>wallType</t>
+  </si>
+  <si>
+    <t>woodType</t>
+  </si>
+  <si>
+    <t>defaultConstructionType</t>
+  </si>
+  <si>
+    <t>Black Stones</t>
+  </si>
+  <si>
+    <t>Absheet</t>
+  </si>
+  <si>
+    <t>BAMBOO</t>
+  </si>
+  <si>
+    <t>Allmixing</t>
+  </si>
+  <si>
+    <t>classificationOfBuilding</t>
+  </si>
+  <si>
+    <t>floorNumber</t>
+  </si>
+  <si>
+    <t>natureOfUsage</t>
+  </si>
+  <si>
+    <t>firmName</t>
+  </si>
+  <si>
+    <t>occupancy</t>
+  </si>
+  <si>
+    <t>occupantName</t>
+  </si>
+  <si>
+    <t>constructionDate</t>
+  </si>
+  <si>
+    <t>firstFloor</t>
+  </si>
+  <si>
+    <t>Huts</t>
+  </si>
+  <si>
+    <t>1st floor</t>
+  </si>
+  <si>
+    <t>Residence</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>effectiveFromDate</t>
+  </si>
+  <si>
+    <t>unstructuredLand</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>breadth</t>
+  </si>
+  <si>
+    <t>buildingPermissionNumber</t>
+  </si>
+  <si>
+    <t>buildingPermissionDate</t>
+  </si>
+  <si>
+    <t>plinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>11/22</t>
+  </si>
+  <si>
+    <t>approverDepartment</t>
+  </si>
+  <si>
+    <t>approverDesignation</t>
+  </si>
+  <si>
+    <t>approver</t>
+  </si>
+  <si>
+    <t>approverRemarks</t>
+  </si>
+  <si>
+    <t>REVENUE</t>
+  </si>
+  <si>
+    <t>Bill Collector</t>
+  </si>
+  <si>
+    <t>D.Khasim ~ REV_Bill Collector_1</t>
+  </si>
+  <si>
+    <t>defaultApprover</t>
+  </si>
+  <si>
+    <t>Forward to BC</t>
   </si>
 </sst>
 </file>
@@ -720,7 +843,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -770,7 +893,7 @@
         <v>123</v>
       </c>
       <c r="F2" s="7">
-        <v>41620</v>
+        <v>42350</v>
       </c>
     </row>
   </sheetData>
@@ -782,7 +905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -846,6 +969,237 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="7">
+        <v>42653</v>
+      </c>
+      <c r="I2" s="7">
+        <v>42654</v>
+      </c>
+      <c r="J2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>20</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="N2" s="7">
+        <v>42358</v>
+      </c>
+      <c r="O2">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>

<commit_message>
create new property all the way till commissioner approval
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/TestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="107">
   <si>
     <t>dataName</t>
   </si>
@@ -298,27 +298,75 @@
     <t>D.Khasim ~ REV_Bill Collector_1</t>
   </si>
   <si>
-    <t>defaultApprover</t>
-  </si>
-  <si>
-    <t>Forward to BC</t>
+    <t>billCollector</t>
+  </si>
+  <si>
+    <t>0944206</t>
+  </si>
+  <si>
+    <t>revenueInspector</t>
+  </si>
+  <si>
+    <t>944210</t>
+  </si>
+  <si>
+    <t>revenueOfficer</t>
+  </si>
+  <si>
+    <t>commissioner</t>
+  </si>
+  <si>
+    <t>946800</t>
+  </si>
+  <si>
+    <t>0935528</t>
+  </si>
+  <si>
+    <t>Forward to bill collector</t>
+  </si>
+  <si>
+    <t>UD Revenue Inspector</t>
+  </si>
+  <si>
+    <t>P.Sadiq Hussain ~ UD RI</t>
+  </si>
+  <si>
+    <t>Forward to revenue officer</t>
+  </si>
+  <si>
+    <t>Revenue Officer</t>
+  </si>
+  <si>
+    <t>B.Veeraswamy ~ REV_Revenue Officer_3</t>
+  </si>
+  <si>
+    <t>Forward to commissioner</t>
+  </si>
+  <si>
+    <t>hasZone</t>
+  </si>
+  <si>
+    <t>ADMINISTRATION</t>
+  </si>
+  <si>
+    <t>Commissioner</t>
+  </si>
+  <si>
+    <t>S.Ravindra Babu ~ ADM_Commissioner_1</t>
+  </si>
+  <si>
+    <t>Forward to revenue insoector</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF008000"/>
-      <name val="Menlo"/>
     </font>
     <font>
       <u/>
@@ -351,18 +399,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -641,20 +688,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="5" customWidth="1"/>
-    <col min="3" max="26" width="10.5" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="4" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,7 +712,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -674,7 +724,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -684,7 +734,9 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="E2" s="2"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -693,6 +745,62 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -751,7 +859,7 @@
       <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F2" t="s">
@@ -784,7 +892,7 @@
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -806,7 +914,7 @@
       <c r="F1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H1" t="s">
@@ -826,7 +934,7 @@
       <c r="F2" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H2">
@@ -892,7 +1000,7 @@
       <c r="E2">
         <v>123</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>42350</v>
       </c>
     </row>
@@ -918,7 +1026,7 @@
       <c r="B1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>43</v>
       </c>
       <c r="D1" t="s">
@@ -1024,7 +1132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
@@ -1039,7 +1147,7 @@
     <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1081,7 +1189,7 @@
       <c r="L1" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>75</v>
       </c>
       <c r="N1" t="s">
@@ -1113,10 +1221,10 @@
       <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="6">
         <v>42653</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="6">
         <v>42654</v>
       </c>
       <c r="J2" t="s">
@@ -1128,10 +1236,10 @@
       <c r="L2">
         <v>20</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="N2" s="7">
+      <c r="N2" s="6">
         <v>42358</v>
       </c>
       <c r="O2">
@@ -1145,10 +1253,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1156,8 +1264,8 @@
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1191,7 +1299,58 @@
         <v>86</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>